<commit_message>
Review Comments of the wireframes are added
Review Comments of the wireframes done by Nessma Bahgat are added to the peer review sheet
</commit_message>
<xml_diff>
--- a/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
+++ b/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nesma Files\ITI\SW Project Management\Travel-Adviser-Web-Application\Review\Peer Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\CM\Travel-Adviser-Web-Application\Review\Peer Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>Deliverable</t>
   </si>
@@ -156,6 +156,16 @@
   </si>
   <si>
     <t>HLD (Design Document)</t>
+  </si>
+  <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
+    <t>1- Add show details button to each trip
+2- The content of the side-bars doesn't exist
+The following screens don't exist:-
+3- What will the user see after submitting the flight?
+4- Where will the user be directed to after signing-up?</t>
   </si>
 </sst>
 </file>
@@ -372,6 +382,10 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -381,10 +395,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -667,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,44 +700,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="1"/>
       <c r="E2" s="3" t="s">
         <v>29</v>
@@ -1092,14 +1102,31 @@
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="F11" s="18">
+      <c r="F11" s="15">
         <v>43595</v>
       </c>
       <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:25" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="15">
+        <v>43743</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Peer review is updated
</commit_message>
<xml_diff>
--- a/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
+++ b/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Deliverable</t>
   </si>
@@ -172,12 +172,16 @@
 2) TAWA_SRS_FR_016 AND TAWA_SRS_FR_066 : email field can contain numbers or characters or both before '@'
 3) TAWA_SRS_FR_134 : Not clear.</t>
   </si>
+  <si>
+    <t>1- Accepted
+2- Rejected : Not necessary</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,8 +248,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +272,11 @@
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -330,11 +346,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,6 +385,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,12 +397,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -661,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Y66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,7 +696,7 @@
     <col min="4" max="4" width="1.33203125" customWidth="1"/>
     <col min="5" max="5" width="48.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
     <col min="8" max="8" width="2.109375" customWidth="1"/>
     <col min="9" max="9" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -685,44 +706,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
     </row>
     <row r="2" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="1"/>
       <c r="E2" s="3" t="s">
         <v>29</v>
@@ -966,7 +987,7 @@
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
     </row>
-    <row r="8" spans="1:25" ht="156.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="141" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
@@ -990,7 +1011,7 @@
       <c r="I8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="15">
         <v>43743</v>
       </c>
       <c r="K8" s="9"/>
@@ -1084,7 +1105,7 @@
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
     </row>
-    <row r="11" spans="1:25" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -1101,6 +1122,9 @@
       <c r="F11" s="14">
         <v>43595</v>
       </c>
+      <c r="G11" s="19" t="s">
+        <v>39</v>
+      </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:25" ht="109.2" x14ac:dyDescent="0.3">
@@ -1122,6 +1146,169 @@
       <c r="G12" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H66" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
review comments had been added on usecase diagram in 'TAWA_PeerReviewSheet.xlsx' document
</commit_message>
<xml_diff>
--- a/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
+++ b/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\TAWA\Travel-Adviser-Web-Application\Review\Peer Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project Management\Project\Travel-Adviser-Web-Application\Review\Peer Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>Deliverable</t>
   </si>
@@ -175,6 +175,15 @@
   <si>
     <t>1- Accepted
 2- Rejected : Not necessary</t>
+  </si>
+  <si>
+    <t>Usecase Diagram</t>
+  </si>
+  <si>
+    <t>Saya Sayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Add usecase for view all users.                                 2- Add usecase for Edit users.                                               3- 'login' usecase include from 'sign up' usecase.       4- Add two usecases 'cash' and 'debit card' and both extend from 'payment' usecase.                                      5- make 'show destination details' include from 'land on photo gallery' usecase.                                     6- make 'explore different airlines' and 'choose payment method' usecase include from 'book flight' usecase.                                                                               </t>
   </si>
 </sst>
 </file>
@@ -351,7 +360,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -388,6 +397,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -397,8 +409,29 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -684,66 +717,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12:H66"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="1.33203125" customWidth="1"/>
-    <col min="5" max="5" width="48.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
-    <col min="8" max="8" width="2.109375" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.6640625" customWidth="1"/>
-    <col min="16" max="16" width="1.5546875" customWidth="1"/>
-    <col min="20" max="20" width="1.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="1.28515625" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.7109375" customWidth="1"/>
+    <col min="16" max="16" width="1.5703125" customWidth="1"/>
+    <col min="20" max="20" width="1.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-    </row>
-    <row r="2" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+    </row>
+    <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="1"/>
       <c r="E2" s="3" t="s">
         <v>29</v>
@@ -797,7 +830,7 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" ht="135.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -835,7 +868,7 @@
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
     </row>
-    <row r="4" spans="1:25" ht="250.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="252.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -873,7 +906,7 @@
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
     </row>
-    <row r="5" spans="1:25" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -911,7 +944,7 @@
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
     </row>
-    <row r="6" spans="1:25" ht="156.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="158.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -949,7 +982,7 @@
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
     </row>
-    <row r="7" spans="1:25" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -987,7 +1020,7 @@
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
     </row>
-    <row r="8" spans="1:25" ht="141" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="158.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
@@ -1014,7 +1047,9 @@
       <c r="J8" s="15">
         <v>43743</v>
       </c>
-      <c r="K8" s="9"/>
+      <c r="K8" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="L8" s="5"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
@@ -1029,7 +1064,7 @@
       <c r="W8" s="9"/>
       <c r="X8" s="9"/>
     </row>
-    <row r="9" spans="1:25" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -1067,14 +1102,14 @@
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
     </row>
-    <row r="10" spans="1:25" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="5"/>
@@ -1105,14 +1140,14 @@
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
     </row>
-    <row r="11" spans="1:25" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="21" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="5"/>
@@ -1122,21 +1157,22 @@
       <c r="F11" s="14">
         <v>43595</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="16" t="s">
         <v>39</v>
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:25" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="111" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="21" t="s">
         <v>14</v>
       </c>
+      <c r="D12" s="5"/>
       <c r="E12" s="11" t="s">
         <v>36</v>
       </c>
@@ -1148,166 +1184,182 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" s="24" customFormat="1" ht="159.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="27">
+        <v>43743</v>
+      </c>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H42" s="5"/>
     </row>
-    <row r="43" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H49" s="5"/>
     </row>
-    <row r="50" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H59" s="5"/>
     </row>
-    <row r="60" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H61" s="5"/>
     </row>
-    <row r="62" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H63" s="5"/>
     </row>
-    <row r="64" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H64" s="5"/>
     </row>
-    <row r="65" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H65" s="5"/>
     </row>
-    <row r="66" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H66" s="5"/>
     </row>
   </sheetData>
@@ -1318,5 +1370,6 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add class diagram review comments
</commit_message>
<xml_diff>
--- a/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
+++ b/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project Management\Project\Travel-Adviser-Web-Application\Review\Peer Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maysoon\Desktop\ProjectManagement\Travel-Adviser-Web-Application\Review\Peer Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8805"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t>Deliverable</t>
   </si>
@@ -184,6 +184,14 @@
   </si>
   <si>
     <t>1- Add usecase for view all users.                                 2- Add usecase for Edit users.                                               3- 'login' usecase include from 'sign up' usecase.       4- Add two usecases 'cash' and 'debit card' and both extend from 'payment' usecase.                                      5- make 'show destination details' include from 'land on photo gallery' usecase.                                     6- make 'explore different airlines' and 'choose payment method' usecase include from 'book flight' usecase.                                                                              7- Add usecase For each airline extend from 'explore different airlines' usecse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class Diagram </t>
+  </si>
+  <si>
+    <t>1- Guest class has (land on top travels / see destination details)_x000D_
+2- login interface class that implements by user and admin_x000D_
+3- Traveler has (Land on destination)</t>
   </si>
 </sst>
 </file>
@@ -289,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -354,13 +362,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -406,18 +442,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -432,6 +462,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -717,66 +768,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="1.28515625" customWidth="1"/>
-    <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="2.140625" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.7109375" customWidth="1"/>
-    <col min="16" max="16" width="1.5703125" customWidth="1"/>
-    <col min="20" max="20" width="1.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="1.33203125" customWidth="1"/>
+    <col min="5" max="5" width="48.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
+    <col min="8" max="8" width="2.109375" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.6640625" customWidth="1"/>
+    <col min="16" max="16" width="1.5546875" customWidth="1"/>
+    <col min="20" max="20" width="1.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:25" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-    </row>
-    <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+    </row>
+    <row r="2" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="1"/>
       <c r="E2" s="3" t="s">
         <v>29</v>
@@ -830,7 +881,7 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="135.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -868,7 +919,7 @@
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
     </row>
-    <row r="4" spans="1:25" ht="252.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="250.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -906,7 +957,7 @@
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
     </row>
-    <row r="5" spans="1:25" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -944,7 +995,7 @@
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
     </row>
-    <row r="6" spans="1:25" ht="158.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="156.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -982,7 +1033,7 @@
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
     </row>
-    <row r="7" spans="1:25" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -1020,7 +1071,7 @@
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
     </row>
-    <row r="8" spans="1:25" ht="174" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
@@ -1064,7 +1115,7 @@
       <c r="W8" s="9"/>
       <c r="X8" s="9"/>
     </row>
-    <row r="9" spans="1:25" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1153,7 @@
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
     </row>
-    <row r="10" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -1140,7 +1191,7 @@
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
     </row>
-    <row r="11" spans="1:25" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -1162,7 +1213,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:25" ht="111" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>35</v>
       </c>
@@ -1184,182 +1235,205 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:25" s="21" customFormat="1" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:25" s="20" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="23" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="22">
         <v>43743</v>
       </c>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="31">
+        <v>43743</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>32</v>
+      </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C15" s="13"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H42" s="5"/>
     </row>
-    <row r="43" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H49" s="5"/>
     </row>
-    <row r="50" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H59" s="5"/>
     </row>
-    <row r="60" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H61" s="5"/>
     </row>
-    <row r="62" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H63" s="5"/>
     </row>
-    <row r="64" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H64" s="5"/>
     </row>
-    <row r="65" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H65" s="5"/>
     </row>
-    <row r="66" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H66" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add reviews for UI and Backend
</commit_message>
<xml_diff>
--- a/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
+++ b/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project Management\Project\Travel-Adviser-Web-Application\Review\Peer Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nesma Files\ITI\SW Project Management\New folder\htdocs\Travel-Adviser-Web-Application\Review\Peer Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
   <si>
     <t>Deliverable</t>
   </si>
@@ -184,6 +184,116 @@
   </si>
   <si>
     <t>1- Add usecase for view all users.                                 2- Add usecase for Edit users.                                               3- 'login' usecase include from 'sign up' usecase.       4- Add two usecases 'cash' and 'debit card' and both extend from 'payment' usecase.                                      5- make 'show destination details' include from 'land on photo gallery' usecase.                                     6- make 'explore different airlines' and 'choose payment method' usecase include from 'book flight' usecase.                                                                              7- Add usecase For each airline extend from 'explore different airlines' usecse.</t>
+  </si>
+  <si>
+    <t>Admin Module (UI)</t>
+  </si>
+  <si>
+    <t>Login Module (UI)</t>
+  </si>
+  <si>
+    <t>Sign up Module (UI)</t>
+  </si>
+  <si>
+    <t>Destination Details Module (UI)</t>
+  </si>
+  <si>
+    <t>Home Page Module(UI)</t>
+  </si>
+  <si>
+    <t>Booking Module (UI)</t>
+  </si>
+  <si>
+    <t>Feedback and Rating Module (UI)</t>
+  </si>
+  <si>
+    <t>Reserved Trips Module (UI)</t>
+  </si>
+  <si>
+    <t>Data Base (BackEnd)</t>
+  </si>
+  <si>
+    <t>Admin Module (BackEnd)</t>
+  </si>
+  <si>
+    <t>Reserved Trips Module (BackEnd)</t>
+  </si>
+  <si>
+    <t>Feedback and Rating Module (BackEnd)</t>
+  </si>
+  <si>
+    <t>Booking Module (BackEnd)</t>
+  </si>
+  <si>
+    <t>Home Page Module(Back End)</t>
+  </si>
+  <si>
+    <t>Destination Details Module (BackEnd)</t>
+  </si>
+  <si>
+    <t>Sign up Module (BackEnd)</t>
+  </si>
+  <si>
+    <t>Login Module (BackEnd)</t>
+  </si>
+  <si>
+    <t>Admin Module (Test Cases)</t>
+  </si>
+  <si>
+    <t>Login Module (Test Cases)</t>
+  </si>
+  <si>
+    <t>Sign up Module (Test cases)</t>
+  </si>
+  <si>
+    <t>Destiantion Details (Test Cases)</t>
+  </si>
+  <si>
+    <t>Home Page (Test Cases)</t>
+  </si>
+  <si>
+    <t>Feedback and rating (Test Cases)</t>
+  </si>
+  <si>
+    <t>Reserved Trips (Test Cases)</t>
+  </si>
+  <si>
+    <t>Booking Module(Test Cases)</t>
+  </si>
+  <si>
+    <t>Page Header (Test Cases)</t>
+  </si>
+  <si>
+    <t>1-Change Font in page.</t>
+  </si>
+  <si>
+    <t>1-Change Font in page.
+2-Field debit Card number should appear only in case user choose debit card as a payment Method</t>
+  </si>
+  <si>
+    <t>1- Stars in Rating is just an image and it must retreive data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Accepted
+2- Rejected : It is done in different way </t>
+  </si>
+  <si>
+    <t>Asmaa Hamdy,Sara Sayed</t>
+  </si>
+  <si>
+    <t>1-change Backgroung.</t>
+  </si>
+  <si>
+    <t>1-Change size of page.
+2-Add required Validation to the page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1-Remove feedbacklink from Header.
+2-Remove the extra Header as there is 2 headers in the page</t>
+  </si>
+  <si>
+    <t>1-Change add user Page style.
+2-In admin page, replace the (edit,delete) buttons at the end of the users name list with 2  buttons for add &amp;delete beside each user name.</t>
   </si>
 </sst>
 </file>
@@ -289,7 +399,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -354,33 +464,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -393,10 +508,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -424,14 +535,32 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -717,650 +846,942 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="1.28515625" customWidth="1"/>
-    <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="2.140625" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.7109375" customWidth="1"/>
-    <col min="16" max="16" width="1.5703125" customWidth="1"/>
-    <col min="20" max="20" width="1.5703125" customWidth="1"/>
+    <col min="1" max="1" width="36" style="13" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="1.28515625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="54" style="13" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.7109375" style="13" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" style="13"/>
+    <col min="16" max="16" width="1.5703125" style="13" customWidth="1"/>
+    <col min="17" max="19" width="9.140625" style="13"/>
+    <col min="20" max="20" width="1.5703125" style="13" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="25" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="3" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="21"/>
+      <c r="I2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="L2" s="21"/>
+      <c r="M2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3" t="s">
+      <c r="T2" s="21"/>
+      <c r="U2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-    </row>
-    <row r="3" spans="1:25" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+    </row>
+    <row r="3" spans="1:25" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="23">
         <v>43470</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-    </row>
-    <row r="4" spans="1:25" ht="252.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+    </row>
+    <row r="4" spans="1:25" ht="237" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="23">
         <v>43470</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
     </row>
     <row r="5" spans="1:25" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="23">
         <v>43470</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
     </row>
     <row r="6" spans="1:25" ht="158.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="23">
         <v>43470</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-    </row>
-    <row r="7" spans="1:25" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+    </row>
+    <row r="7" spans="1:25" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="12" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="23">
         <v>43501</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
     </row>
     <row r="8" spans="1:25" ht="174" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="11" t="s">
+      <c r="H8" s="12"/>
+      <c r="I8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="16">
         <v>43743</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-    </row>
-    <row r="9" spans="1:25" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="L8" s="12"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+    </row>
+    <row r="9" spans="1:25" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="12"/>
+      <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-    </row>
-    <row r="10" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="H9" s="12"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+    </row>
+    <row r="10" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="11" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
     </row>
     <row r="11" spans="1:25" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="24">
         <v>43595</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:25" ht="111" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:25" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="11" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="24">
         <v>43743</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:25" s="21" customFormat="1" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:25" ht="200.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="23" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="16">
         <v>43743</v>
       </c>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H48" s="5"/>
+      <c r="G13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:25" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="24">
+        <v>43601</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="24">
+        <v>43601</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="24">
+        <v>43601</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="24">
+        <v>43601</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="24">
+        <v>43600</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="24">
+        <v>43600</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="24">
+        <v>43600</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="12"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="12"/>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="12"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="12"/>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="12"/>
+      <c r="H25" s="12"/>
+    </row>
+    <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="12"/>
+      <c r="H26" s="12"/>
+    </row>
+    <row r="27" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="12"/>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="12"/>
+      <c r="H28" s="12"/>
+    </row>
+    <row r="29" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="12"/>
+      <c r="H29" s="12"/>
+    </row>
+    <row r="30" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="12"/>
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="12"/>
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="12"/>
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="12"/>
+      <c r="H33" s="12"/>
+    </row>
+    <row r="34" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="12"/>
+      <c r="H34" s="12"/>
+    </row>
+    <row r="35" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="12"/>
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="12"/>
+      <c r="H36" s="12"/>
+    </row>
+    <row r="37" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="12"/>
+      <c r="H37" s="12"/>
+    </row>
+    <row r="38" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="12"/>
+      <c r="H38" s="12"/>
+    </row>
+    <row r="39" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="12"/>
+      <c r="H39" s="12"/>
+    </row>
+    <row r="40" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="14"/>
+      <c r="H40" s="12"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H41" s="12"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H42" s="12"/>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H43" s="12"/>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H44" s="12"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H45" s="12"/>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H46" s="12"/>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H47" s="12"/>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H48" s="12"/>
     </row>
     <row r="49" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H49" s="5"/>
+      <c r="H49" s="12"/>
     </row>
     <row r="50" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H50" s="5"/>
+      <c r="H50" s="12"/>
     </row>
     <row r="51" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H51" s="5"/>
+      <c r="H51" s="12"/>
     </row>
     <row r="52" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H52" s="5"/>
+      <c r="H52" s="12"/>
     </row>
     <row r="53" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H53" s="5"/>
+      <c r="H53" s="12"/>
     </row>
     <row r="54" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H54" s="5"/>
+      <c r="H54" s="12"/>
     </row>
     <row r="55" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H55" s="5"/>
+      <c r="H55" s="12"/>
     </row>
     <row r="56" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H56" s="5"/>
+      <c r="H56" s="12"/>
     </row>
     <row r="57" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H57" s="5"/>
+      <c r="H57" s="12"/>
     </row>
     <row r="58" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H58" s="5"/>
+      <c r="H58" s="12"/>
     </row>
     <row r="59" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H59" s="5"/>
+      <c r="H59" s="12"/>
     </row>
     <row r="60" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H60" s="5"/>
+      <c r="H60" s="12"/>
     </row>
     <row r="61" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H61" s="5"/>
+      <c r="H61" s="12"/>
     </row>
     <row r="62" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H62" s="5"/>
+      <c r="H62" s="12"/>
     </row>
     <row r="63" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H63" s="5"/>
+      <c r="H63" s="12"/>
     </row>
     <row r="64" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H64" s="5"/>
+      <c r="H64" s="12"/>
     </row>
     <row r="65" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H65" s="5"/>
+      <c r="H65" s="12"/>
     </row>
     <row r="66" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H66" s="5"/>
+      <c r="H66" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Peer Review sheet is updated
Peer Review sheet is updatedwith the reviews of the back-end of the admin module and the testcases of the login module
</commit_message>
<xml_diff>
--- a/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
+++ b/Review/Peer Review/TAWA_PeerReviewSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nesma Files\ITI\SW Project Management\New folder\htdocs\Travel-Adviser-Web-Application\Review\Peer Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\CM\Travel-Adviser-Web-Application\Review\Peer Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
   <si>
     <t>Deliverable</t>
   </si>
@@ -294,6 +294,25 @@
   <si>
     <t>1-Change add user Page style.
 2-In admin page, replace the (edit,delete) buttons at the end of the users name list with 2  buttons for add &amp;delete beside each user name.</t>
+  </si>
+  <si>
+    <t>1- Testcases Status should be passed or failed 
+2-The expected result of the error message after wrong user name or password should be "wrong username or password"</t>
+  </si>
+  <si>
+    <t>23/5/2019</t>
+  </si>
+  <si>
+    <t>1- The fields in the edit user page shouldn't be empty
+2-There should be a logout function in the admin page
+3-The buttons of the edit and delete should be seperated for each user</t>
+  </si>
+  <si>
+    <t>1, 2 Accepted
+3 Rejected</t>
+  </si>
+  <si>
+    <t>21/5/2019</t>
   </si>
 </sst>
 </file>
@@ -375,7 +394,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -485,7 +510,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -535,32 +560,35 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -846,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,96 +899,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="21" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21" t="s">
+      <c r="L2" s="18"/>
+      <c r="M2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21" t="s">
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="R2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="S2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21" t="s">
+      <c r="T2" s="18"/>
+      <c r="U2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="21" t="s">
+      <c r="W2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
     </row>
     <row r="3" spans="1:25" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -976,7 +1004,7 @@
       <c r="E3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>43470</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1014,7 +1042,7 @@
       <c r="E4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>43470</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1052,7 +1080,7 @@
       <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <v>43470</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -1090,7 +1118,7 @@
       <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <v>43470</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -1128,7 +1156,7 @@
       <c r="E7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <v>43501</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -1166,7 +1194,7 @@
       <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="20" t="s">
         <v>31</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -1210,7 +1238,7 @@
       <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="20" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -1248,7 +1276,7 @@
       <c r="E10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="20" t="s">
         <v>31</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -1286,7 +1314,7 @@
       <c r="E11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="21">
         <v>43595</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -1308,7 +1336,7 @@
       <c r="E12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="21">
         <v>43743</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -1352,7 +1380,7 @@
       <c r="E14" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="21">
         <v>43601</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -1361,7 +1389,7 @@
       <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -1374,7 +1402,7 @@
       <c r="E15" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="21">
         <v>43601</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -1383,7 +1411,7 @@
       <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -1396,7 +1424,7 @@
       <c r="E16" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="21">
         <v>43601</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -1405,7 +1433,7 @@
       <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="22" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="11" t="s">
@@ -1418,7 +1446,7 @@
       <c r="E17" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="24">
+      <c r="F17" s="21">
         <v>43601</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -1427,7 +1455,7 @@
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -1440,7 +1468,7 @@
       <c r="E18" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="24">
+      <c r="F18" s="21">
         <v>43600</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1449,7 +1477,7 @@
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -1462,7 +1490,7 @@
       <c r="E19" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="21">
         <v>43600</v>
       </c>
       <c r="G19" s="8" t="s">
@@ -1471,7 +1499,7 @@
       <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="11" t="s">
@@ -1484,7 +1512,7 @@
       <c r="E20" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="21">
         <v>43600</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -1493,7 +1521,7 @@
       <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="22" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -1504,7 +1532,7 @@
       <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="22" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="11" t="s">
@@ -1514,19 +1542,30 @@
       <c r="D22" s="12"/>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+    <row r="23" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="14"/>
+      <c r="C23" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="D23" s="12"/>
+      <c r="E23" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>81</v>
+      </c>
       <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="22" t="s">
         <v>59</v>
       </c>
       <c r="B24" s="11" t="s">
@@ -1537,7 +1576,7 @@
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="22" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="11" t="s">
@@ -1548,7 +1587,7 @@
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="22" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -1559,7 +1598,7 @@
       <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="22" t="s">
         <v>56</v>
       </c>
       <c r="B27" s="11" t="s">
@@ -1570,7 +1609,7 @@
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B28" s="11" t="s">
@@ -1581,7 +1620,7 @@
       <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="22" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="11" t="s">
@@ -1592,7 +1631,7 @@
       <c r="H29" s="12"/>
     </row>
     <row r="30" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B30" s="11" t="s">
@@ -1603,7 +1642,7 @@
       <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="22" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="11" t="s">
@@ -1613,19 +1652,30 @@
       <c r="D31" s="12"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="25" t="s">
+    <row r="32" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="22" t="s">
         <v>61</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="14"/>
+      <c r="C32" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="D32" s="12"/>
+      <c r="E32" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>32</v>
+      </c>
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="22" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="11" t="s">
@@ -1636,7 +1686,7 @@
       <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="22" t="s">
         <v>63</v>
       </c>
       <c r="B34" s="11" t="s">
@@ -1647,7 +1697,7 @@
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="22" t="s">
         <v>64</v>
       </c>
       <c r="B35" s="11" t="s">
@@ -1658,7 +1708,7 @@
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="22" t="s">
         <v>65</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -1669,7 +1719,7 @@
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="22" t="s">
         <v>66</v>
       </c>
       <c r="B37" s="11" t="s">
@@ -1680,7 +1730,7 @@
       <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="22" t="s">
         <v>67</v>
       </c>
       <c r="B38" s="11" t="s">
@@ -1691,7 +1741,7 @@
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="22" t="s">
         <v>68</v>
       </c>
       <c r="B39" s="11" t="s">

</xml_diff>